<commit_message>
Wrote some more in evaluation.
</commit_message>
<xml_diff>
--- a/Models/analysis.xlsx
+++ b/Models/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875DD325-4950-4823-9A10-D9FAB5B14064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACD0529-55D1-4BB7-900D-3751CFB81BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="2655" windowWidth="21405" windowHeight="15435" firstSheet="4" activeTab="6" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
@@ -2489,6 +2489,18 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>2.4813000000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.4599000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.4563999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.4510000000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.4409999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26307,7 +26319,7 @@
   <dimension ref="A2:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26902,32 +26914,54 @@
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="6"/>
-      <c r="C44" s="8"/>
+      <c r="B44" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="C44" s="8">
+        <v>2.4599000000000002</v>
+      </c>
       <c r="D44" s="8"/>
       <c r="E44" s="3"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="6"/>
-      <c r="C45" s="8"/>
+      <c r="B45" s="6">
+        <v>1.23</v>
+      </c>
+      <c r="C45" s="8">
+        <v>2.4563999999999999</v>
+      </c>
       <c r="D45" s="8"/>
       <c r="E45" s="3"/>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="6"/>
-      <c r="C46" s="8"/>
+      <c r="B46" s="6">
+        <v>1.26</v>
+      </c>
+      <c r="C46" s="8">
+        <v>2.4510000000000001</v>
+      </c>
       <c r="D46" s="8"/>
       <c r="E46" s="3"/>
       <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="6"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="10"/>
+      <c r="B47" s="6">
+        <v>1.29</v>
+      </c>
+      <c r="C47" s="8">
+        <v>2.4409999999999998</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.15609999999999999</v>
+      </c>
+      <c r="F47" s="10">
+        <v>0.14940000000000001</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>

</xml_diff>

<commit_message>
Rewrote first evaluation section.
</commit_message>
<xml_diff>
--- a/Models/analysis.xlsx
+++ b/Models/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5A3716-1C65-4E5B-A554-BD3FB1583B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C66571-8778-4BD4-8DBE-D7F9791C2600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="2655" windowWidth="21405" windowHeight="15435" activeTab="4" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="6540" yWindow="2655" windowWidth="21405" windowHeight="15435" activeTab="5" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT_EN" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="22">
   <si>
     <t>Language</t>
   </si>
@@ -1334,172 +1334,91 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>7.5202</c:v>
+                  <c:v>7.4960000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9242999999999997</c:v>
+                  <c:v>6.9497</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6300999999999997</c:v>
+                  <c:v>6.8319000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8022999999999998</c:v>
+                  <c:v>6.6040999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3838999999999997</c:v>
+                  <c:v>6.5033000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9266000000000001</c:v>
+                  <c:v>6.4447999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6959</c:v>
+                  <c:v>6.3974000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4697</c:v>
+                  <c:v>6.3483000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2985000000000002</c:v>
+                  <c:v>6.3299000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1602999999999999</c:v>
+                  <c:v>6.2938000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0687000000000002</c:v>
+                  <c:v>6.2617000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9903</c:v>
+                  <c:v>6.2569999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9287000000000001</c:v>
+                  <c:v>6.2206000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.8708</c:v>
+                  <c:v>6.2111999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.8323</c:v>
+                  <c:v>6.1917999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.7966000000000002</c:v>
+                  <c:v>6.1458000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.7627000000000002</c:v>
+                  <c:v>6.1070000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.7221000000000002</c:v>
+                  <c:v>5.9507000000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.6871999999999998</c:v>
+                  <c:v>5.8789999999999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.6004</c:v>
+                  <c:v>5.8007999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5912000000000002</c:v>
+                  <c:v>5.7188999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.5857000000000001</c:v>
+                  <c:v>5.4748000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.5714000000000001</c:v>
+                  <c:v>5.2538999999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.5421999999999998</c:v>
+                  <c:v>5.1193</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.5308000000000002</c:v>
+                  <c:v>5.0026999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.5230000000000001</c:v>
+                  <c:v>4.9242999999999997</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5063</c:v>
+                  <c:v>4.8148999999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.5017</c:v>
+                  <c:v>4.7233000000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4834999999999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.4828999999999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.4693999999999998</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.4597000000000002</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.4338000000000002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2.4388000000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.4236</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.4068999999999998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2.4156</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2.3431000000000002</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2.2862</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2.2843</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.2866</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.2732999999999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2.2894000000000001</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2.2637999999999998</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2.2669000000000001</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2.2595999999999998</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2.2530999999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2.2643</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2.2545999999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2.2416999999999998</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.2256999999999998</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2.2317999999999998</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2.234</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2.2290000000000001</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2.2252999999999998</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2.2136999999999998</c:v>
+                  <c:v>4.6189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1786,7 +1705,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
-            <c:idx val="0"/>
+            <c:idx val="1"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -1802,42 +1721,16 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-DD14-4166-90D8-66C2F2EAF7C8}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-DD14-4166-90D8-66C2F2EAF7C8}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="2"/>
+            <c:idx val="3"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-DD14-4166-90D8-66C2F2EAF7C8}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1853,24 +1746,21 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR_DE!$D$12,XLMR_DE!$D$22,XLMR_DE!$D$32,XLMR_DE!$D$42,XLMR_DE!$D$52)</c:f>
+              <c:f>(XLMR_DE!$D$7,XLMR_DE!$D$12,XLMR_DE!$D$17,XLMR_DE!$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.1400000000000005E-2</c:v>
+                  <c:v>4.1000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7600000000000006E-2</c:v>
+                  <c:v>7.1999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9500000000000005E-2</c:v>
+                  <c:v>8.0999999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1084</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1099</c:v>
+                  <c:v>1.23E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1909,7 +1799,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
-            <c:idx val="0"/>
+            <c:idx val="1"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -1923,53 +1813,24 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-DD14-4166-90D8-66C2F2EAF7C8}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-DD14-4166-90D8-66C2F2EAF7C8}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR_DE!$E$12,XLMR_DE!$E$22,XLMR_DE!$E$32,XLMR_DE!$E$42,XLMR_DE!$E$52)</c:f>
+              <c:f>(XLMR_DE!$E$7,XLMR_DE!$E$12,XLMR_DE!$E$17,XLMR_DE!$E$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1192</c:v>
+                  <c:v>5.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15570000000000001</c:v>
+                  <c:v>1.03E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15820000000000001</c:v>
+                  <c:v>1.15E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1694</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.17150000000000001</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1977,7 +1838,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-B9B8-4352-B83D-6F7A5C87D675}"/>
+              <c16:uniqueId val="{0000000F-EA91-41EC-92B0-2A402871FFEA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2008,7 +1869,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
-            <c:idx val="0"/>
+            <c:idx val="1"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -2022,53 +1883,24 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-DD14-4166-90D8-66C2F2EAF7C8}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-DD14-4166-90D8-66C2F2EAF7C8}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR_DE!$F$12,XLMR_DE!$F$22,XLMR_DE!$F$32,XLMR_DE!$F$42,XLMR_DE!$F$52)</c:f>
+              <c:f>(XLMR_DE!$F$7,XLMR_DE!$F$12,XLMR_DE!$F$17,XLMR_DE!$F$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.43E-2</c:v>
+                  <c:v>4.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1135</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11550000000000001</c:v>
+                  <c:v>8.8999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12520000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.12670000000000001</c:v>
+                  <c:v>1.2699999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2076,7 +1908,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-B9B8-4352-B83D-6F7A5C87D675}"/>
+              <c16:uniqueId val="{00000010-EA91-41EC-92B0-2A402871FFEA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18806,8 +18638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8D7B0E-2744-461D-949E-D223AB56EB6D}">
   <dimension ref="A2:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19555,8 +19387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42CEBC-4DF1-4EAE-9662-1F6C023E63EA}">
   <dimension ref="A2:I59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19592,7 +19424,7 @@
         <v>0.05</v>
       </c>
       <c r="C3" s="7">
-        <v>7.5202</v>
+        <v>7.4960000000000004</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
@@ -19609,7 +19441,7 @@
         <v>0.11</v>
       </c>
       <c r="C4" s="8">
-        <v>6.9242999999999997</v>
+        <v>6.9497</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="3"/>
@@ -19627,7 +19459,7 @@
         <v>0.16</v>
       </c>
       <c r="C5" s="8">
-        <v>6.6300999999999997</v>
+        <v>6.8319000000000001</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="3"/>
@@ -19645,7 +19477,7 @@
         <v>0.21</v>
       </c>
       <c r="C6" s="8">
-        <v>5.8022999999999998</v>
+        <v>6.6040999999999999</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="3"/>
@@ -19663,11 +19495,17 @@
         <v>0.27</v>
       </c>
       <c r="C7" s="8">
-        <v>4.3838999999999997</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
+        <v>6.5033000000000003</v>
+      </c>
+      <c r="D7" s="8">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5.3E-3</v>
+      </c>
+      <c r="F7" s="10">
+        <v>4.3E-3</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
         <v>13</v>
@@ -19681,7 +19519,7 @@
         <v>0.32</v>
       </c>
       <c r="C8" s="8">
-        <v>3.9266000000000001</v>
+        <v>6.4447999999999999</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="3"/>
@@ -19693,7 +19531,7 @@
         <v>0.37</v>
       </c>
       <c r="C9" s="8">
-        <v>3.6959</v>
+        <v>6.3974000000000002</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="3"/>
@@ -19705,7 +19543,7 @@
         <v>0.43</v>
       </c>
       <c r="C10" s="8">
-        <v>3.4697</v>
+        <v>6.3483000000000001</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="3"/>
@@ -19718,7 +19556,7 @@
         <v>0.48</v>
       </c>
       <c r="C11" s="8">
-        <v>3.2985000000000002</v>
+        <v>6.3299000000000003</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="3"/>
@@ -19730,16 +19568,16 @@
         <v>0.53</v>
       </c>
       <c r="C12" s="8">
-        <v>3.1602999999999999</v>
+        <v>6.2938000000000001</v>
       </c>
       <c r="D12" s="8">
-        <v>7.1400000000000005E-2</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="E12" s="3">
-        <v>0.1192</v>
+        <v>1.03E-2</v>
       </c>
       <c r="F12" s="10">
-        <v>8.43E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -19748,7 +19586,7 @@
         <v>0.59</v>
       </c>
       <c r="C13" s="8">
-        <v>3.0687000000000002</v>
+        <v>6.2617000000000003</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="3"/>
@@ -19760,7 +19598,7 @@
         <v>0.64</v>
       </c>
       <c r="C14" s="8">
-        <v>2.9903</v>
+        <v>6.2569999999999997</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="3"/>
@@ -19772,7 +19610,7 @@
         <v>0.69</v>
       </c>
       <c r="C15" s="8">
-        <v>2.9287000000000001</v>
+        <v>6.2206000000000001</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="3"/>
@@ -19784,7 +19622,7 @@
         <v>0.75</v>
       </c>
       <c r="C16" s="8">
-        <v>2.8708</v>
+        <v>6.2111999999999998</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="3"/>
@@ -19796,11 +19634,17 @@
         <v>0.8</v>
       </c>
       <c r="C17" s="8">
-        <v>2.8323</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="10"/>
+        <v>6.1917999999999997</v>
+      </c>
+      <c r="D17" s="8">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.15E-2</v>
+      </c>
+      <c r="F17" s="10">
+        <v>8.8999999999999999E-3</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -19808,7 +19652,7 @@
         <v>0.85</v>
       </c>
       <c r="C18" s="8">
-        <v>2.7966000000000002</v>
+        <v>6.1458000000000004</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="3"/>
@@ -19820,7 +19664,7 @@
         <v>0.91</v>
       </c>
       <c r="C19" s="8">
-        <v>2.7627000000000002</v>
+        <v>6.1070000000000002</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
@@ -19832,7 +19676,7 @@
         <v>0.96</v>
       </c>
       <c r="C20" s="8">
-        <v>2.7221000000000002</v>
+        <v>5.9507000000000003</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>
@@ -19844,7 +19688,7 @@
         <v>1.01</v>
       </c>
       <c r="C21" s="8">
-        <v>2.6871999999999998</v>
+        <v>5.8789999999999996</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="3"/>
@@ -19856,16 +19700,16 @@
         <v>1.07</v>
       </c>
       <c r="C22" s="8">
-        <v>2.6004</v>
+        <v>5.8007999999999997</v>
       </c>
       <c r="D22" s="8">
-        <v>9.7600000000000006E-2</v>
+        <v>1.23E-2</v>
       </c>
       <c r="E22" s="3">
-        <v>0.15570000000000001</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F22" s="10">
-        <v>0.1135</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -19874,7 +19718,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="C23" s="8">
-        <v>2.5912000000000002</v>
+        <v>5.7188999999999997</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="3"/>
@@ -19886,7 +19730,7 @@
         <v>1.17</v>
       </c>
       <c r="C24" s="8">
-        <v>2.5857000000000001</v>
+        <v>5.4748000000000001</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="3"/>
@@ -19898,7 +19742,7 @@
         <v>1.23</v>
       </c>
       <c r="C25" s="8">
-        <v>2.5714000000000001</v>
+        <v>5.2538999999999998</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="3"/>
@@ -19910,7 +19754,7 @@
         <v>1.28</v>
       </c>
       <c r="C26" s="8">
-        <v>2.5421999999999998</v>
+        <v>5.1193</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="3"/>
@@ -19922,11 +19766,17 @@
         <v>1.33</v>
       </c>
       <c r="C27" s="8">
-        <v>2.5308000000000002</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="10"/>
+        <v>5.0026999999999999</v>
+      </c>
+      <c r="D27" s="8">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="F27" s="10">
+        <v>3.09E-2</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -19934,7 +19784,7 @@
         <v>1.39</v>
       </c>
       <c r="C28" s="8">
-        <v>2.5230000000000001</v>
+        <v>4.9242999999999997</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="3"/>
@@ -19946,7 +19796,7 @@
         <v>1.44</v>
       </c>
       <c r="C29" s="8">
-        <v>2.5063</v>
+        <v>4.8148999999999997</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="3"/>
@@ -19958,7 +19808,7 @@
         <v>1.49</v>
       </c>
       <c r="C30" s="8">
-        <v>2.5017</v>
+        <v>4.7233000000000001</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="3"/>
@@ -19970,7 +19820,7 @@
         <v>1.55</v>
       </c>
       <c r="C31" s="8">
-        <v>2.4834999999999998</v>
+        <v>4.6189</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="3"/>
@@ -19979,320 +19829,194 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="C32" s="8">
-        <v>2.4828999999999999</v>
-      </c>
-      <c r="D32" s="8">
-        <v>9.9500000000000005E-2</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.15820000000000001</v>
-      </c>
-      <c r="F32" s="10">
-        <v>0.11550000000000001</v>
-      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="6">
-        <v>1.65</v>
-      </c>
-      <c r="C33" s="8">
-        <v>2.4693999999999998</v>
-      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="3"/>
       <c r="F33" s="10"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="6">
-        <v>1.71</v>
-      </c>
-      <c r="C34" s="8">
-        <v>2.4597000000000002</v>
-      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="3"/>
       <c r="F34" s="10"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="6">
-        <v>1.76</v>
-      </c>
-      <c r="C35" s="8">
-        <v>2.4338000000000002</v>
-      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="3"/>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="6">
-        <v>1.81</v>
-      </c>
-      <c r="C36" s="8">
-        <v>2.4388000000000001</v>
-      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="3"/>
       <c r="F36" s="10"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="6">
-        <v>1.87</v>
-      </c>
-      <c r="C37" s="8">
-        <v>2.4236</v>
-      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="3"/>
       <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="6">
-        <v>1.92</v>
-      </c>
-      <c r="C38" s="8">
-        <v>2.4068999999999998</v>
-      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="3"/>
       <c r="F38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="6">
-        <v>1.97</v>
-      </c>
-      <c r="C39" s="8">
-        <v>2.4156</v>
-      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="3"/>
       <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="6">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="C40" s="8">
-        <v>2.3431000000000002</v>
-      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="3"/>
       <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="6">
-        <v>2.08</v>
-      </c>
-      <c r="C41" s="8">
-        <v>2.2862</v>
-      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="3"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="6">
-        <v>2.13</v>
-      </c>
-      <c r="C42" s="8">
-        <v>2.2843</v>
-      </c>
-      <c r="D42" s="8">
-        <v>0.1084</v>
-      </c>
-      <c r="E42" s="3">
-        <v>0.1694</v>
-      </c>
-      <c r="F42" s="10">
-        <v>0.12520000000000001</v>
-      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="6">
-        <v>2.19</v>
-      </c>
-      <c r="C43" s="8">
-        <v>2.2866</v>
-      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="3"/>
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="6">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="C44" s="8">
-        <v>2.2732999999999999</v>
-      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="3"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
-        <v>2.29</v>
-      </c>
-      <c r="C45" s="8">
-        <v>2.2894000000000001</v>
-      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="3"/>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="6">
-        <v>2.35</v>
-      </c>
-      <c r="C46" s="8">
-        <v>2.2637999999999998</v>
-      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="3"/>
       <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="C47" s="8">
-        <v>2.2669000000000001</v>
-      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="3"/>
       <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="6">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="C48" s="8">
-        <v>2.2595999999999998</v>
-      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="3"/>
       <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="6">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="C49" s="8">
-        <v>2.2530999999999999</v>
-      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="3"/>
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="6">
-        <v>2.56</v>
-      </c>
-      <c r="C50" s="8">
-        <v>2.2643</v>
-      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="3"/>
       <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="6">
-        <v>2.61</v>
-      </c>
-      <c r="C51" s="8">
-        <v>2.2545999999999999</v>
-      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="3"/>
       <c r="F51" s="10"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="6">
-        <v>2.67</v>
-      </c>
-      <c r="C52" s="8">
-        <v>2.2416999999999998</v>
-      </c>
-      <c r="D52" s="8">
-        <v>0.1099</v>
-      </c>
-      <c r="E52" s="3">
-        <v>0.17150000000000001</v>
-      </c>
-      <c r="F52" s="10">
-        <v>0.12670000000000001</v>
-      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="10"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="6">
-        <v>2.72</v>
-      </c>
-      <c r="C53" s="8">
-        <v>2.2256999999999998</v>
-      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="3"/>
       <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="6">
-        <v>2.77</v>
-      </c>
-      <c r="C54" s="8">
-        <v>2.2317999999999998</v>
-      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="3"/>
       <c r="F54" s="10"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="6">
-        <v>2.83</v>
-      </c>
-      <c r="C55" s="8">
-        <v>2.234</v>
-      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="3"/>
       <c r="F55" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="6">
-        <v>2.88</v>
-      </c>
-      <c r="C56" s="8">
-        <v>2.2290000000000001</v>
-      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="3"/>
       <c r="F56" s="10"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="6">
-        <v>2.93</v>
-      </c>
-      <c r="C57" s="8">
-        <v>2.2252999999999998</v>
-      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="3"/>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="6">
-        <v>2.99</v>
-      </c>
-      <c r="C58" s="8">
-        <v>2.2136999999999998</v>
-      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="3"/>
       <c r="F58" s="10"/>
@@ -20301,21 +20025,11 @@
       <c r="A59" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="17">
-        <v>3</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="14">
-        <v>0.1032</v>
-      </c>
-      <c r="E59" s="14">
-        <v>0.1593</v>
-      </c>
-      <c r="F59" s="14">
-        <v>0.1186</v>
-      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>